<commit_message>
Upload Chapter 17 - Domestic Violence
Upload of code to produce domestic violence indicators from Chapter 17 of the Guide to DHS Statistics
</commit_message>
<xml_diff>
--- a/DHS7tabplan/Tab_plan_Chap17_Domestic_Violence.xlsx
+++ b/DHS7tabplan/Tab_plan_Chap17_Domestic_Violence.xlsx
@@ -17995,7 +17995,7 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="481" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="be21cae339529f0f311ef097f4a87693">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A3299ADD5D91FC4981A62029954D61DA" ma:contentTypeVersion="533" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9fe6dd6fbc47b2b2c3033f1a9c1079fd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd" xmlns:ns3="d16efad5-0601-4cf0-b7c2-89968258c777" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fd9e5a0c56088652e9b5d1a36fcd7f8a" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="aa3c2c9a-d70f-4174-bdeb-29973d8fe5cd"/>
@@ -18300,5 +18300,5 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E687B041-5352-4277-9F94-472B91D2ADAD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37378340-9C52-4125-8E59-32F3F3F541E9}"/>
 </file>
</xml_diff>